<commit_message>
add second module to boot camp 2 course
</commit_message>
<xml_diff>
--- a/inst/Courses/Mathematical_Biostatistics_Boot_Camp_2/Module1.xlsx
+++ b/inst/Courses/Mathematical_Biostatistics_Boot_Camp_2/Module1.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Dropbox\R_Working_Directory\My_Packages\swirl\inst\Boot_Camp_Modules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Dropbox\swirl_shared\Boot Camp 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8340"/>
+    <workbookView xWindow="12405" yWindow="765" windowWidth="15360" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,12 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A:$L</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -63,9 +68,6 @@
     <t>In this module, I'm going to walk you through a one sample t-test step-by-step using the 'mtcars' dataset. This dataset comes built in to R and gives a series of design and performance characteristics for 32 car models built in 1973-74.</t>
   </si>
   <si>
-    <t>Once you learn the one sample t-test procedure, I will have you complete a second t-test analysis on your own using a different dataset. If you get stuck, there will be hints along the way.</t>
-  </si>
-  <si>
     <t>Let's begin by taking a look at the 'mtcars' dataset. Type 'mtcars' without quotes and press Enter.</t>
   </si>
   <si>
@@ -186,9 +188,6 @@
     <t>Let's take a look at what's stored in 'allMPG'. Typing a variable's name and pressing Enter will print its contents to the console.</t>
   </si>
   <si>
-    <t>Before moving on to our final calculations, let's view the contents of the variables involved. Remember that typing a variables name and pressing Enter will show you the contents of that variable.</t>
-  </si>
-  <si>
     <t>Compute the degrees of freedom by storing the value 'n - 1' in a new variable called 'myDF'.</t>
   </si>
   <si>
@@ -234,12 +233,6 @@
     <t>Let's compute the area under the curve to the right of our t-statistic using R's 'pt' function. In case you're wondering, the 'p' in 'pt' stands for 'probability' and the 't' stands for 't-distribution'.</t>
   </si>
   <si>
-    <t>pVal &lt;- pt(tStat, df = df, lower.tail=FALSE)'</t>
-  </si>
-  <si>
-    <t>Type 'pVal &lt;- pt(tStat, df = df, lower.tail=FALSE)' and press Enter.</t>
-  </si>
-  <si>
     <t>Type the following to compute the probability of getting a t-statistic that's greater than the value of the one we got: 'pVal &lt;- pt(tStat, df = df, lower.tail=FALSE)'</t>
   </si>
   <si>
@@ -265,13 +258,25 @@
   </si>
   <si>
     <t>Success!!! Your p-values are equal! In the future, using the 't.test' function will save you time and reduce your chances of making a computational error. However, it's important for you to understand the calculations behind the t-test procedure, so that you properly interpret the results.</t>
+  </si>
+  <si>
+    <t>Once you learn the one sample t-test procedure, I will have you complete a second t-test analysis on your own using the same dataset. If you get stuck, there will be hints along the way.</t>
+  </si>
+  <si>
+    <t>Before moving on to our final calculations, let's view the contents of the variables involved. Remember that typing a variable's name and pressing Enter will show you the contents of that variable.</t>
+  </si>
+  <si>
+    <t>pVal &lt;- pt(tStat, df = myDF, lower.tail=FALSE)'</t>
+  </si>
+  <si>
+    <t>Type 'pVal &lt;- pt(tStat, df = myDF, lower.tail=FALSE)' and press Enter.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -295,6 +300,12 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="5">
@@ -333,23 +344,31 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -377,7 +396,15 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="10">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -718,7 +745,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -753,7 +780,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -943,21 +970,21 @@
   </sheetPr>
   <dimension ref="A1:Q131"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="75.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="33.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="20.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="28.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="28.7109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="34.28515625" style="1" customWidth="1"/>
-    <col min="8" max="9" width="32.5703125" style="1" customWidth="1"/>
+    <col min="8" max="9" width="32.42578125" style="1" customWidth="1"/>
     <col min="10" max="11" width="33" style="4" customWidth="1"/>
     <col min="12" max="12" width="57.140625" style="2" customWidth="1"/>
     <col min="13" max="13" width="28.7109375" style="1" hidden="1" customWidth="1"/>
@@ -973,7 +1000,7 @@
         <v>5</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>7</v>
@@ -997,7 +1024,7 @@
         <v>3</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>4</v>
@@ -1018,7 +1045,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -1028,7 +1055,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -1038,16 +1065,16 @@
         <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -1057,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -1067,7 +1094,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -1077,16 +1104,16 @@
         <v>11</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -1096,7 +1123,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -1106,7 +1133,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -1116,16 +1143,16 @@
         <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -1135,7 +1162,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -1145,16 +1172,16 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -1164,7 +1191,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -1174,16 +1201,16 @@
         <v>11</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
@@ -1193,7 +1220,7 @@
         <v>10</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -1203,16 +1230,16 @@
         <v>11</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -1222,7 +1249,7 @@
         <v>10</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
@@ -1232,16 +1259,16 @@
         <v>11</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F19" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
@@ -1251,7 +1278,7 @@
         <v>10</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
@@ -1261,16 +1288,16 @@
         <v>11</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
@@ -1280,7 +1307,7 @@
         <v>10</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
@@ -1290,16 +1317,16 @@
         <v>11</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
@@ -1309,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
@@ -1319,16 +1346,16 @@
         <v>11</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F25" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
@@ -1338,16 +1365,16 @@
         <v>11</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
@@ -1357,7 +1384,7 @@
         <v>10</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
@@ -1367,7 +1394,7 @@
         <v>10</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C28" s="6"/>
       <c r="J28" s="1"/>
@@ -1378,16 +1405,16 @@
         <v>11</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
@@ -1397,7 +1424,7 @@
         <v>10</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
@@ -1407,16 +1434,16 @@
         <v>11</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G31" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
@@ -1426,16 +1453,16 @@
         <v>11</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
@@ -1445,7 +1472,7 @@
         <v>10</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
@@ -1455,7 +1482,7 @@
         <v>10</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
@@ -1465,7 +1492,7 @@
         <v>10</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
@@ -1475,16 +1502,16 @@
         <v>11</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
@@ -1494,7 +1521,7 @@
         <v>10</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
@@ -2017,6 +2044,11 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="37" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="37" fitToHeight="0" orientation="landscape"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add first half of 3rd boot camp module and a few fixes to first two modules
</commit_message>
<xml_diff>
--- a/inst/Courses/Mathematical_Biostatistics_Boot_Camp_2/Module1.xlsx
+++ b/inst/Courses/Mathematical_Biostatistics_Boot_Camp_2/Module1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Dropbox\swirl_shared\Boot Camp 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Dropbox\R_Working_Directory\My_Packages\swirl\inst\Courses\Mathematical_Biostatistics_Boot_Camp_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -155,18 +155,9 @@
     <t>Recall that a t-statistic is computed by subtracting the population mean from the sample mean and dividing that quantity by the square root of the sample variance over n. This is difficult to express in words, but very easy to compute.</t>
   </si>
   <si>
-    <t>Store the following quantity in a new variable called 'tStat': '(sampMeanMPG - 24.7) / sqrt(sampVarMPG/n)'.</t>
-  </si>
-  <si>
     <t>If you are new to R, the '&lt;-' is called an assignment operator and is just a 'less than' sign followed by a dash, with no space in between. It is customary that you include a space before and after the assignment operator. You can think of the assignment operator as an 'equals' sign since it just assigns the value on its right to the variable on its left.</t>
   </si>
   <si>
-    <t>tStat &lt;- (sampMeanMPG - 24.7) / sqrt(sampVarMPG/n)</t>
-  </si>
-  <si>
-    <t>Type 'tStat &lt;- (sampMeanMPG - 24.7) / sqrt(sampVarMPG/n)' to store the value of our t-statistic in a new variable called 'tStat'.</t>
-  </si>
-  <si>
     <t>Now that we have our t-statistic, we must compare it to our t critical value. In order to do this, we need to specify the t distribution corresponding to the correct degrees of freedom (which equals n - 1).</t>
   </si>
   <si>
@@ -233,9 +224,6 @@
     <t>Let's compute the area under the curve to the right of our t-statistic using R's 'pt' function. In case you're wondering, the 'p' in 'pt' stands for 'probability' and the 't' stands for 't-distribution'.</t>
   </si>
   <si>
-    <t>Type the following to compute the probability of getting a t-statistic that's greater than the value of the one we got: 'pVal &lt;- pt(tStat, df = df, lower.tail=FALSE)'</t>
-  </si>
-  <si>
     <t>To reiterate, the variable 'pVal' now stores the probability of getting a t-statistic greater than or equal to the one we got. However, since we are interested in both extremes (i.e. a two-sided test), we must multiply this probability by 2 to get our official p-value!</t>
   </si>
   <si>
@@ -266,10 +254,22 @@
     <t>Before moving on to our final calculations, let's view the contents of the variables involved. Remember that typing a variable's name and pressing Enter will show you the contents of that variable.</t>
   </si>
   <si>
-    <t>pVal &lt;- pt(tStat, df = myDF, lower.tail=FALSE)'</t>
-  </si>
-  <si>
     <t>Type 'pVal &lt;- pt(tStat, df = myDF, lower.tail=FALSE)' and press Enter.</t>
+  </si>
+  <si>
+    <t>Store the following quantity in a new variable called 'tStat': '(sampMeanMPG - 12.0) / sqrt(sampVarMPG/n)'.</t>
+  </si>
+  <si>
+    <t>tStat &lt;- (sampMeanMPG - 12.0) / sqrt(sampVarMPG/n)</t>
+  </si>
+  <si>
+    <t>Type 'tStat &lt;- (sampMeanMPG - 12.0) / sqrt(sampVarMPG/n)' to store the value of our t-statistic in a new variable called 'tStat'.</t>
+  </si>
+  <si>
+    <t>Type the following to compute the probability of getting a t-statistic that's greater than the value of the one we got: 'pVal &lt;- pt(tStat, df = myDF, lower.tail=FALSE)'</t>
+  </si>
+  <si>
+    <t>pVal &lt;- pt(tStat, df = myDF, lower.tail=FALSE)</t>
   </si>
 </sst>
 </file>
@@ -970,9 +970,9 @@
   </sheetPr>
   <dimension ref="A1:Q131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1000,7 +1000,7 @@
         <v>5</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>7</v>
@@ -1045,7 +1045,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -1123,7 +1123,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -1143,16 +1143,16 @@
         <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -1288,16 +1288,16 @@
         <v>11</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
@@ -1307,7 +1307,7 @@
         <v>10</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
@@ -1317,16 +1317,16 @@
         <v>11</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
@@ -1336,7 +1336,7 @@
         <v>10</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
@@ -1346,16 +1346,16 @@
         <v>11</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
@@ -1365,16 +1365,16 @@
         <v>11</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
@@ -1384,7 +1384,7 @@
         <v>10</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
@@ -1394,7 +1394,7 @@
         <v>10</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C28" s="6"/>
       <c r="J28" s="1"/>
@@ -1405,16 +1405,16 @@
         <v>11</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
@@ -1424,7 +1424,7 @@
         <v>10</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
@@ -1434,16 +1434,16 @@
         <v>11</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
@@ -1453,16 +1453,16 @@
         <v>11</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
@@ -1472,7 +1472,7 @@
         <v>10</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
@@ -1482,7 +1482,7 @@
         <v>10</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
@@ -1492,7 +1492,7 @@
         <v>10</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
@@ -1502,16 +1502,16 @@
         <v>11</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
@@ -1521,7 +1521,7 @@
         <v>10</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>

</xml_diff>

<commit_message>
debugged boot camp 2 modules further and altered interpretation of double quote in correct answer - also fixed progress bar bug
</commit_message>
<xml_diff>
--- a/inst/Courses/Mathematical_Biostatistics_Boot_Camp_2/Module1.xlsx
+++ b/inst/Courses/Mathematical_Biostatistics_Boot_Camp_2/Module1.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="22810"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Dropbox\R_Working_Directory\My_Packages\swirl\inst\Courses\Mathematical_Biostatistics_Boot_Camp_2\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12405" yWindow="765" windowWidth="15360" windowHeight="8340"/>
+    <workbookView xWindow="8300" yWindow="2560" windowWidth="19440" windowHeight="10780"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -957,7 +952,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -965,34 +960,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:Q131"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="75.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="33.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="28.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="28.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="34.28515625" style="1" customWidth="1"/>
-    <col min="8" max="9" width="32.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="75.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="33.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="28.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="28.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="34.33203125" style="1" customWidth="1"/>
+    <col min="8" max="9" width="32.5" style="1" customWidth="1"/>
     <col min="10" max="11" width="33" style="4" customWidth="1"/>
-    <col min="12" max="12" width="57.140625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="28.7109375" style="1" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="57.1640625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="28.6640625" style="1" hidden="1" customWidth="1"/>
     <col min="14" max="17" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="18" max="16384" width="28.7109375" style="1" hidden="1"/>
+    <col min="18" max="16384" width="28.6640625" style="1" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="5" customFormat="1" ht="17">
       <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
@@ -1030,7 +1025,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="60" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="45">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -1040,7 +1035,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:12" ht="45" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="45">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1050,7 +1045,7 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:12" ht="45" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="45">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1060,7 +1055,7 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="30">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -1079,7 +1074,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:12" ht="105" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="90">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1089,7 +1084,7 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:12" ht="90" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="75">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1099,7 +1094,7 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:12" ht="60" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="45">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -1118,7 +1113,7 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:12" ht="75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="75">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -1128,7 +1123,7 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="45">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1138,7 +1133,7 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="30">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -1157,7 +1152,7 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="30">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1167,7 +1162,7 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:12" ht="60" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="60">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1186,7 +1181,7 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:12" ht="60" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="60">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -1196,7 +1191,7 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:12" ht="60" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="60">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
@@ -1215,7 +1210,7 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:12" ht="45" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="45">
       <c r="A16" s="1" t="s">
         <v>10</v>
       </c>
@@ -1225,7 +1220,7 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11" ht="60" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="60">
       <c r="A17" s="1" t="s">
         <v>11</v>
       </c>
@@ -1244,7 +1239,7 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11" ht="60" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="60">
       <c r="A18" s="1" t="s">
         <v>10</v>
       </c>
@@ -1254,7 +1249,7 @@
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="45">
       <c r="A19" s="1" t="s">
         <v>11</v>
       </c>
@@ -1273,7 +1268,7 @@
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11" ht="60" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="45">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
@@ -1283,7 +1278,7 @@
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="1:11" ht="60" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="60">
       <c r="A21" s="1" t="s">
         <v>11</v>
       </c>
@@ -1302,7 +1297,7 @@
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="45">
       <c r="A22" s="1" t="s">
         <v>10</v>
       </c>
@@ -1312,7 +1307,7 @@
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="30">
       <c r="A23" s="1" t="s">
         <v>11</v>
       </c>
@@ -1331,7 +1326,7 @@
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="45">
       <c r="A24" s="1" t="s">
         <v>10</v>
       </c>
@@ -1341,7 +1336,7 @@
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11">
       <c r="A25" s="1" t="s">
         <v>11</v>
       </c>
@@ -1360,7 +1355,7 @@
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11">
       <c r="A26" s="1" t="s">
         <v>11</v>
       </c>
@@ -1379,7 +1374,7 @@
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="1:11" ht="90" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="75">
       <c r="A27" s="1" t="s">
         <v>10</v>
       </c>
@@ -1389,7 +1384,7 @@
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="45">
       <c r="A28" s="1" t="s">
         <v>10</v>
       </c>
@@ -1400,7 +1395,7 @@
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="30">
       <c r="A29" s="1" t="s">
         <v>11</v>
       </c>
@@ -1419,7 +1414,7 @@
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="1:11" ht="60" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" ht="60">
       <c r="A30" s="1" t="s">
         <v>10</v>
       </c>
@@ -1429,7 +1424,7 @@
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="1:11" ht="60" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" ht="45">
       <c r="A31" s="1" t="s">
         <v>11</v>
       </c>
@@ -1448,7 +1443,7 @@
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11">
       <c r="A32" s="1" t="s">
         <v>11</v>
       </c>
@@ -1467,7 +1462,7 @@
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="1:11" ht="75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" ht="60">
       <c r="A33" s="1" t="s">
         <v>10</v>
       </c>
@@ -1477,7 +1472,7 @@
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="1:11" ht="60" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" ht="60">
       <c r="A34" s="1" t="s">
         <v>10</v>
       </c>
@@ -1487,7 +1482,7 @@
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="1:11" ht="75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" ht="60">
       <c r="A35" s="1" t="s">
         <v>10</v>
       </c>
@@ -1497,7 +1492,7 @@
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="1:11" ht="75" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" ht="60">
       <c r="A36" s="1" t="s">
         <v>11</v>
       </c>
@@ -1516,7 +1511,7 @@
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
     </row>
-    <row r="37" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" ht="75" customHeight="1">
       <c r="A37" s="1" t="s">
         <v>10</v>
       </c>
@@ -1526,379 +1521,379 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11">
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11">
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11">
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11">
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11">
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11">
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11">
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11">
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11">
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11">
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11">
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
     </row>
-    <row r="49" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="10:11">
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
     </row>
-    <row r="50" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="10:11">
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
     </row>
-    <row r="51" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="10:11">
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
     </row>
-    <row r="52" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="10:11">
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
     </row>
-    <row r="53" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="10:11">
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
     </row>
-    <row r="54" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="10:11">
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
     </row>
-    <row r="55" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="10:11">
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
     </row>
-    <row r="56" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="10:11">
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
     </row>
-    <row r="57" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="10:11">
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
     </row>
-    <row r="58" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="10:11">
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
     </row>
-    <row r="59" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="10:11">
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
     </row>
-    <row r="60" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="10:11">
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
     </row>
-    <row r="61" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="10:11">
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
     </row>
-    <row r="62" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="10:11">
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
     </row>
-    <row r="63" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="10:11">
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
     </row>
-    <row r="64" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="10:11">
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
     </row>
-    <row r="65" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="65" spans="10:11">
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
     </row>
-    <row r="66" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="66" spans="10:11">
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
     </row>
-    <row r="67" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="67" spans="10:11">
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
     </row>
-    <row r="68" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="68" spans="10:11">
       <c r="J68" s="1"/>
       <c r="K68" s="1"/>
     </row>
-    <row r="69" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="69" spans="10:11">
       <c r="J69" s="1"/>
       <c r="K69" s="1"/>
     </row>
-    <row r="70" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="70" spans="10:11">
       <c r="J70" s="1"/>
       <c r="K70" s="1"/>
     </row>
-    <row r="71" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="71" spans="10:11">
       <c r="J71" s="1"/>
       <c r="K71" s="1"/>
     </row>
-    <row r="72" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="72" spans="10:11">
       <c r="J72" s="1"/>
       <c r="K72" s="1"/>
     </row>
-    <row r="73" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="73" spans="10:11">
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
     </row>
-    <row r="74" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="74" spans="10:11">
       <c r="J74" s="1"/>
       <c r="K74" s="1"/>
     </row>
-    <row r="75" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="75" spans="10:11">
       <c r="J75" s="1"/>
       <c r="K75" s="1"/>
     </row>
-    <row r="76" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="76" spans="10:11">
       <c r="J76" s="1"/>
       <c r="K76" s="1"/>
     </row>
-    <row r="77" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="77" spans="10:11">
       <c r="J77" s="1"/>
       <c r="K77" s="1"/>
     </row>
-    <row r="78" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="78" spans="10:11">
       <c r="J78" s="1"/>
       <c r="K78" s="1"/>
     </row>
-    <row r="79" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="79" spans="10:11">
       <c r="J79" s="1"/>
       <c r="K79" s="1"/>
     </row>
-    <row r="80" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="80" spans="10:11">
       <c r="J80" s="1"/>
       <c r="K80" s="1"/>
     </row>
-    <row r="81" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="81" spans="10:11">
       <c r="J81" s="1"/>
       <c r="K81" s="1"/>
     </row>
-    <row r="82" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="82" spans="10:11">
       <c r="J82" s="1"/>
       <c r="K82" s="1"/>
     </row>
-    <row r="83" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="83" spans="10:11">
       <c r="J83" s="1"/>
       <c r="K83" s="1"/>
     </row>
-    <row r="84" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="84" spans="10:11">
       <c r="J84" s="1"/>
       <c r="K84" s="1"/>
     </row>
-    <row r="85" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="85" spans="10:11">
       <c r="J85" s="1"/>
       <c r="K85" s="1"/>
     </row>
-    <row r="86" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="86" spans="10:11">
       <c r="J86" s="1"/>
       <c r="K86" s="1"/>
     </row>
-    <row r="87" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="87" spans="10:11">
       <c r="J87" s="1"/>
       <c r="K87" s="1"/>
     </row>
-    <row r="88" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="88" spans="10:11">
       <c r="J88" s="1"/>
       <c r="K88" s="1"/>
     </row>
-    <row r="89" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="89" spans="10:11">
       <c r="J89" s="1"/>
       <c r="K89" s="1"/>
     </row>
-    <row r="90" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="90" spans="10:11">
       <c r="J90" s="1"/>
       <c r="K90" s="1"/>
     </row>
-    <row r="91" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="91" spans="10:11">
       <c r="J91" s="1"/>
       <c r="K91" s="1"/>
     </row>
-    <row r="92" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="92" spans="10:11">
       <c r="J92" s="1"/>
       <c r="K92" s="1"/>
     </row>
-    <row r="93" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="93" spans="10:11">
       <c r="J93" s="1"/>
       <c r="K93" s="1"/>
     </row>
-    <row r="94" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="94" spans="10:11">
       <c r="J94" s="1"/>
       <c r="K94" s="1"/>
     </row>
-    <row r="95" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="95" spans="10:11">
       <c r="J95" s="3"/>
       <c r="K95" s="3"/>
     </row>
-    <row r="96" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="96" spans="10:11">
       <c r="J96" s="1"/>
       <c r="K96" s="1"/>
     </row>
-    <row r="97" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="97" spans="10:11">
       <c r="J97" s="1"/>
       <c r="K97" s="1"/>
     </row>
-    <row r="98" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="98" spans="10:11">
       <c r="J98" s="1"/>
       <c r="K98" s="1"/>
     </row>
-    <row r="99" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="99" spans="10:11">
       <c r="J99" s="1"/>
       <c r="K99" s="1"/>
     </row>
-    <row r="100" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="100" spans="10:11">
       <c r="J100" s="1"/>
       <c r="K100" s="1"/>
     </row>
-    <row r="101" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="101" spans="10:11">
       <c r="J101" s="1"/>
       <c r="K101" s="1"/>
     </row>
-    <row r="102" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="102" spans="10:11">
       <c r="J102" s="1"/>
       <c r="K102" s="1"/>
     </row>
-    <row r="103" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="103" spans="10:11">
       <c r="J103" s="1"/>
       <c r="K103" s="1"/>
     </row>
-    <row r="104" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="104" spans="10:11">
       <c r="J104" s="1"/>
       <c r="K104" s="1"/>
     </row>
-    <row r="105" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="105" spans="10:11">
       <c r="J105" s="1"/>
       <c r="K105" s="1"/>
     </row>
-    <row r="106" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="106" spans="10:11">
       <c r="J106" s="1"/>
       <c r="K106" s="1"/>
     </row>
-    <row r="107" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="107" spans="10:11">
       <c r="J107" s="1"/>
       <c r="K107" s="1"/>
     </row>
-    <row r="108" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="108" spans="10:11">
       <c r="J108" s="1"/>
       <c r="K108" s="1"/>
     </row>
-    <row r="109" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="109" spans="10:11">
       <c r="J109" s="1"/>
       <c r="K109" s="1"/>
     </row>
-    <row r="110" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="110" spans="10:11">
       <c r="J110" s="1"/>
       <c r="K110" s="1"/>
     </row>
-    <row r="111" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="111" spans="10:11">
       <c r="J111" s="1"/>
       <c r="K111" s="1"/>
     </row>
-    <row r="112" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="112" spans="10:11">
       <c r="J112" s="1"/>
       <c r="K112" s="1"/>
     </row>
-    <row r="113" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="113" spans="10:11">
       <c r="J113" s="1"/>
       <c r="K113" s="1"/>
     </row>
-    <row r="114" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="114" spans="10:11">
       <c r="J114" s="1"/>
       <c r="K114" s="1"/>
     </row>
-    <row r="115" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="115" spans="10:11">
       <c r="J115" s="1"/>
       <c r="K115" s="1"/>
     </row>
-    <row r="116" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="116" spans="10:11">
       <c r="J116" s="1"/>
       <c r="K116" s="1"/>
     </row>
-    <row r="117" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="117" spans="10:11">
       <c r="J117" s="1"/>
       <c r="K117" s="1"/>
     </row>
-    <row r="118" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="118" spans="10:11">
       <c r="J118" s="1"/>
       <c r="K118" s="1"/>
     </row>
-    <row r="119" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="119" spans="10:11">
       <c r="J119" s="1"/>
       <c r="K119" s="1"/>
     </row>
-    <row r="120" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="120" spans="10:11">
       <c r="J120" s="1"/>
       <c r="K120" s="1"/>
     </row>
-    <row r="121" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="121" spans="10:11">
       <c r="J121" s="1"/>
       <c r="K121" s="1"/>
     </row>
-    <row r="122" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="122" spans="10:11">
       <c r="J122" s="1"/>
       <c r="K122" s="1"/>
     </row>
-    <row r="123" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="123" spans="10:11">
       <c r="J123" s="1"/>
       <c r="K123" s="1"/>
     </row>
-    <row r="124" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="124" spans="10:11">
       <c r="J124" s="1"/>
       <c r="K124" s="1"/>
     </row>
-    <row r="125" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="125" spans="10:11">
       <c r="J125" s="1"/>
       <c r="K125" s="1"/>
     </row>
-    <row r="126" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="126" spans="10:11">
       <c r="J126" s="1"/>
       <c r="K126" s="1"/>
     </row>
-    <row r="127" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="127" spans="10:11">
       <c r="J127" s="1"/>
       <c r="K127" s="1"/>
     </row>
-    <row r="128" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="128" spans="10:11">
       <c r="J128" s="1"/>
       <c r="K128" s="1"/>
     </row>
-    <row r="129" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="129" spans="10:11">
       <c r="J129" s="1"/>
       <c r="K129" s="1"/>
     </row>
-    <row r="130" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="130" spans="10:11">
       <c r="J130" s="1"/>
       <c r="K130" s="1"/>
     </row>
-    <row r="131" spans="10:11" x14ac:dyDescent="0.2">
+    <row r="131" spans="10:11">
       <c r="J131" s="1"/>
       <c r="K131" s="1"/>
     </row>

</xml_diff>